<commit_message>
slip gaji per file
</commit_message>
<xml_diff>
--- a/kwitansi_output/Details_Miftahul_Arifin_19Jan-22Jan2023.xlsx
+++ b/kwitansi_output/Details_Miftahul_Arifin_19Jan-22Jan2023.xlsx
@@ -745,7 +745,7 @@
       </c>
       <c r="AA2" t="inlineStr">
         <is>
-          <t>5 Tahun 1 Bulan 27 Hari</t>
+          <t>5 Tahun 2 Bulan 0 Hari</t>
         </is>
       </c>
       <c r="AB2" t="n">
@@ -901,7 +901,7 @@
       </c>
       <c r="AA3" t="inlineStr">
         <is>
-          <t>5 Tahun 1 Bulan 27 Hari</t>
+          <t>5 Tahun 2 Bulan 0 Hari</t>
         </is>
       </c>
       <c r="AB3" t="n">
@@ -1057,7 +1057,7 @@
       </c>
       <c r="AA4" t="inlineStr">
         <is>
-          <t>5 Tahun 1 Bulan 27 Hari</t>
+          <t>5 Tahun 2 Bulan 0 Hari</t>
         </is>
       </c>
       <c r="AB4" t="n">
@@ -1215,7 +1215,7 @@
       </c>
       <c r="AA5" s="2" t="inlineStr">
         <is>
-          <t>5 Tahun 1 Bulan 27 Hari</t>
+          <t>5 Tahun 2 Bulan 0 Hari</t>
         </is>
       </c>
       <c r="AB5" s="2" t="n">

</xml_diff>